<commit_message>
Fixing and update to digisales mobile version 2
</commit_message>
<xml_diff>
--- a/DocTest/Error-Digisales New.xlsx
+++ b/DocTest/Error-Digisales New.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\1442\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\1427\Documents\BNI\DigiSales\DocTest\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{C071872F-AF5C-40BB-9123-D2991A7A09B6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{363AA4BE-2D95-4E7E-BF19-B0DBFC531736}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{BFFC41F5-A5FC-4EB8-8594-690B7726E68F}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="20">
   <si>
     <t>Note Rombakan</t>
   </si>
@@ -73,18 +73,47 @@
     <t>SCD0172</t>
   </si>
   <si>
-    <t>1. Sebelum Search Refresh Halaman Terlebih Dahulu
+    <t>SCD0174</t>
+  </si>
+  <si>
+    <t>1. Buka Dedicated dan Free dalam 1 iterasi harus menambahkan fungsi back</t>
+  </si>
+  <si>
+    <t>SCD0175</t>
+  </si>
+  <si>
+    <t>1. Konfirmasi ketika add cart dari 3x menjadi 2x
+2. Setiap buka Dedicated, Free, Kelolaan, dan Prospek harus menambahkan fungsi back dulu</t>
+  </si>
+  <si>
+    <t>SCD0176</t>
+  </si>
+  <si>
+    <t>1. Sebelum Search, Refresh Halaman Terlebih Dahulu
 2. Data Saat Proses Dedicated Tidak Dapat Di Search</t>
+  </si>
+  <si>
+    <t>1. Setiap Search di Dedicated, Free, Kelolaan, dan Prospek Store, Refresh Halaman Terlebih Dahulu
+2. Data Saat Proses di Pipeline Tidak Dapat Di Search, harus klik btn refresh terlebih dahulu</t>
+  </si>
+  <si>
+    <t>SCD0177</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -141,7 +170,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -149,6 +178,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -156,16 +188,16 @@
   <dxfs count="2">
     <dxf>
       <border outline="0">
-        <bottom style="medium">
+        <top style="medium">
           <color indexed="64"/>
-        </bottom>
+        </top>
       </border>
     </dxf>
     <dxf>
       <border outline="0">
-        <top style="medium">
+        <bottom style="medium">
           <color indexed="64"/>
-        </top>
+        </bottom>
       </border>
     </dxf>
   </dxfs>
@@ -182,7 +214,7 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{662B73DA-1A8B-471B-87BE-CCF492A885E6}" name="Table3" displayName="Table3" ref="A1:C12" totalsRowShown="0" headerRowBorderDxfId="0" tableBorderDxfId="1">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{662B73DA-1A8B-471B-87BE-CCF492A885E6}" name="Table3" displayName="Table3" ref="A1:C12" totalsRowShown="0" headerRowBorderDxfId="1" tableBorderDxfId="0">
   <autoFilter ref="A1:C12" xr:uid="{662B73DA-1A8B-471B-87BE-CCF492A885E6}"/>
   <tableColumns count="3">
     <tableColumn id="1" xr3:uid="{7CEE03B5-BCD3-4F53-97B3-DA07DFBCFAEB}" name="Scenario"/>
@@ -490,16 +522,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A6986F4A-47AB-4F08-802D-2F2928085B8A}">
-  <dimension ref="A1:C6"/>
+  <dimension ref="A1:C10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="18.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="72.5703125" customWidth="1"/>
+    <col min="2" max="2" width="69.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -514,7 +546,7 @@
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+      <c r="A2" s="5" t="s">
         <v>2</v>
       </c>
       <c r="B2" s="1" t="s">
@@ -523,7 +555,7 @@
       <c r="C2" s="1"/>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+      <c r="A3" s="5" t="s">
         <v>5</v>
       </c>
       <c r="B3" t="s">
@@ -531,7 +563,7 @@
       </c>
     </row>
     <row r="4" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+      <c r="A4" s="5" t="s">
         <v>7</v>
       </c>
       <c r="B4" s="1" t="s">
@@ -539,7 +571,7 @@
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+      <c r="A5" s="5" t="s">
         <v>9</v>
       </c>
       <c r="B5" t="s">
@@ -547,14 +579,47 @@
       </c>
     </row>
     <row r="6" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+      <c r="A6" s="5" t="s">
         <v>11</v>
       </c>
       <c r="B6" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" s="5" t="s">
         <v>12</v>
       </c>
+      <c r="B7" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+      <c r="A8" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" ht="60" x14ac:dyDescent="0.25">
+      <c r="A9" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" ht="60" x14ac:dyDescent="0.25">
+      <c r="A10" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>18</v>
+      </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">
     <tablePart r:id="rId1"/>

</xml_diff>

<commit_message>
Fixing and update digisales new version
</commit_message>
<xml_diff>
--- a/DocTest/Error-Digisales New.xlsx
+++ b/DocTest/Error-Digisales New.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\1427\Documents\BNI\DigiSales\DocTest\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{363AA4BE-2D95-4E7E-BF19-B0DBFC531736}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CCA98A2D-7378-4496-B684-54CB358CB06C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{BFFC41F5-A5FC-4EB8-8594-690B7726E68F}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="22">
   <si>
     <t>Note Rombakan</t>
   </si>
@@ -98,6 +98,13 @@
   </si>
   <si>
     <t>SCD0177</t>
+  </si>
+  <si>
+    <t>SCD0206-SCD0209</t>
+  </si>
+  <si>
+    <t>1. Button Export Excel nya tidak tersedia
+2. Step Export Excel tidak dapat dilakukan</t>
   </si>
 </sst>
 </file>
@@ -522,10 +529,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A6986F4A-47AB-4F08-802D-2F2928085B8A}">
-  <dimension ref="A1:C10"/>
+  <dimension ref="A1:C11"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -616,6 +623,14 @@
       </c>
       <c r="B10" s="1" t="s">
         <v>18</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A11" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>21</v>
       </c>
     </row>
   </sheetData>

</xml_diff>